<commit_message>
Update timetable generation logic to use new input filename format and improve date handling based on filename. Remove outdated 'flute-time-table.xlsx' file.
</commit_message>
<xml_diff>
--- a/student_timetables/Cybi CHENG_timetable.xlsx
+++ b/student_timetables/Cybi CHENG_timetable.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,48 +432,43 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="7" customWidth="1" min="1" max="1"/>
-    <col width="52" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
-    <col width="44" customWidth="1" min="4" max="4"/>
-    <col width="6" customWidth="1" min="5" max="5"/>
-    <col width="44" customWidth="1" min="6" max="6"/>
-    <col width="6" customWidth="1" min="7" max="7"/>
-    <col width="57" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="9"/>
-    <col width="39" customWidth="1" min="10" max="10"/>
-    <col width="6" customWidth="1" min="11" max="11"/>
-    <col width="78" customWidth="1" min="12" max="12"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="3" max="3"/>
+    <col width="35" customWidth="1" min="4" max="4"/>
+    <col width="35" customWidth="1" min="5" max="5"/>
+    <col width="35" customWidth="1" min="6" max="6"/>
+    <col width="35" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Day 1</t>
+          <t>14 Jul (Monday)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>15 Jul (Tuesday)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Day 2</t>
+          <t>16 Jul (Wednesday)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>17 Jul (Thursday)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Day 3</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Day 4</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Day 5</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Day 6</t>
+          <t>18 Jul (Friday)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>19 Jul (Saturday)</t>
         </is>
       </c>
     </row>
@@ -495,22 +490,22 @@
           <t>Welcome Speech</t>
         </is>
       </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Workshop</t>
+        </is>
+      </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
           <t>Workshop</t>
         </is>
       </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>Workshop</t>
+        </is>
+      </c>
       <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>Workshop</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>Workshop</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
         <is>
           <t>Briefing for Saturday
 (Room zzz)</t>
@@ -523,7 +518,7 @@
           <t>10:15</t>
         </is>
       </c>
-      <c r="L4" s="2" t="inlineStr">
+      <c r="G4" s="2" t="inlineStr">
         <is>
           <t>Check in Maritime Museum
 Briefing for Saturday Concert 
@@ -557,31 +552,31 @@
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>Private lesson with Ivy CHUANG 
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Private Lesson with Ivy CHUANG 
 (Room Ivy)</t>
         </is>
       </c>
-      <c r="H7" s="2" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="J7" s="2" t="inlineStr">
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>Flute MasterClass
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="L7" s="2" t="inlineStr">
+      <c r="G7" s="2" t="inlineStr">
         <is>
           <t>Rehearsal for Students and Friends Concert</t>
         </is>
@@ -614,13 +609,13 @@
           <t>12:00</t>
         </is>
       </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Private Lesson with Ivy CHUANG 
+(Room Ivy)</t>
+        </is>
+      </c>
       <c r="D11" s="2" t="inlineStr">
-        <is>
-          <t>Private lesson with Ivy CHUANG 
-(Room Ivy)</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="inlineStr">
         <is>
           <t>Rehearsal with pianist
 (Room Shelley)</t>
@@ -659,27 +654,27 @@
           <t>Lunch</t>
         </is>
       </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="H15" s="2" t="inlineStr">
-        <is>
-          <t>Lunch</t>
-        </is>
-      </c>
-      <c r="J15" s="2" t="inlineStr">
-        <is>
-          <t>Lunch</t>
-        </is>
-      </c>
-      <c r="L15" s="2" t="inlineStr">
+      <c r="G15" s="2" t="inlineStr">
         <is>
           <t>Lunch
 Dress Up, Warm Up</t>
@@ -715,35 +710,35 @@
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>Private lesson with Stephane RETY 
+          <t>Private Lesson with Stephane RETY 
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="D19" s="2" t="inlineStr">
+      <c r="C19" s="2" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="F19" s="2" t="inlineStr">
+      <c r="D19" s="2" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="H19" s="2" t="inlineStr">
+      <c r="E19" s="2" t="inlineStr">
         <is>
           <t>Private Lesson with Stephane &amp; pianist 
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="J19" s="2" t="inlineStr">
+      <c r="F19" s="2" t="inlineStr">
         <is>
           <t>Flute MasterClass
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="L19" s="3" t="inlineStr">
+      <c r="G19" s="3" t="inlineStr">
         <is>
           <t>Concert call time</t>
         </is>
@@ -755,7 +750,7 @@
           <t>14:15</t>
         </is>
       </c>
-      <c r="L20" s="2" t="inlineStr">
+      <c r="G20" s="2" t="inlineStr">
         <is>
           <t>Lina Summer Camp of Music Students &amp; Friends Concert</t>
         </is>
@@ -787,25 +782,25 @@
 (Room Acting)</t>
         </is>
       </c>
-      <c r="D23" s="2" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>Acting Class 
 (Room Acting)</t>
         </is>
       </c>
-      <c r="F23" s="2" t="inlineStr">
+      <c r="D23" s="2" t="inlineStr">
         <is>
           <t>Acting Class 
 (Room Acting)</t>
         </is>
       </c>
-      <c r="H23" s="2" t="inlineStr">
+      <c r="E23" s="2" t="inlineStr">
         <is>
           <t>Acting Class 
 (Room Acting)</t>
         </is>
       </c>
-      <c r="J23" s="2" t="inlineStr">
+      <c r="F23" s="2" t="inlineStr">
         <is>
           <t>Group Activity 
 (Room Group Activity)</t>
@@ -832,7 +827,7 @@
           <t>15:45</t>
         </is>
       </c>
-      <c r="L26" s="2" t="inlineStr">
+      <c r="G26" s="2" t="inlineStr">
         <is>
           <t>After concert refreshment 
 (Maritime Museum)</t>
@@ -851,25 +846,25 @@
 (Room Tomasz)</t>
         </is>
       </c>
-      <c r="D27" s="2" t="inlineStr">
+      <c r="C27" s="2" t="inlineStr">
         <is>
           <t>Ensemble 
 (Room Tomasz)</t>
         </is>
       </c>
-      <c r="F27" s="2" t="inlineStr">
+      <c r="D27" s="2" t="inlineStr">
         <is>
           <t>Ensemble 
 (Room Tomasz)</t>
         </is>
       </c>
-      <c r="H27" s="2" t="inlineStr">
+      <c r="E27" s="2" t="inlineStr">
         <is>
           <t>Ensemble 
 (Room Tomasz)</t>
         </is>
       </c>
-      <c r="J27" s="2" t="inlineStr">
+      <c r="F27" s="2" t="inlineStr">
         <is>
           <t>Ensemble 
 (Room Tomasz)</t>
@@ -899,43 +894,43 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="L26:L28"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="E7:E14"/>
+    <mergeCell ref="E23:E26"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B14"/>
-    <mergeCell ref="J19:J22"/>
     <mergeCell ref="F15:F18"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="D27:D30"/>
-    <mergeCell ref="J15:J18"/>
-    <mergeCell ref="L15:L18"/>
-    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="G26:G28"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="F3:F6"/>
-    <mergeCell ref="L7:L14"/>
+    <mergeCell ref="F7:F14"/>
+    <mergeCell ref="G7:G14"/>
     <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E15:E18"/>
     <mergeCell ref="B19:B22"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="C27:C30"/>
     <mergeCell ref="F23:F26"/>
-    <mergeCell ref="L20:L25"/>
+    <mergeCell ref="E27:E30"/>
     <mergeCell ref="D3:D6"/>
+    <mergeCell ref="C11:C14"/>
     <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C7:C10"/>
     <mergeCell ref="D15:D18"/>
+    <mergeCell ref="C23:C26"/>
     <mergeCell ref="F27:F30"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="H27:H30"/>
+    <mergeCell ref="C19:C22"/>
     <mergeCell ref="D23:D26"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="H7:H14"/>
-    <mergeCell ref="J3:J6"/>
-    <mergeCell ref="J7:J14"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G20:G25"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D19:D22"/>
     <mergeCell ref="F19:F22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="J23:J26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add border styling to generated timetables for teachers and students, enhancing visual presentation. Update Excel file generation logic to apply consistent cell borders across all timetable sheets.
</commit_message>
<xml_diff>
--- a/student_timetables/Cybi CHENG_timetable.xlsx
+++ b/student_timetables/Cybi CHENG_timetable.xlsx
@@ -37,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,17 +45,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -441,84 +448,97 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>14 Jul (Monday)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>15 Jul (Tuesday)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>16 Jul (Wednesday)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>17 Jul (Thursday)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>18 Jul (Friday)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>19 Jul (Saturday)</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>10:00</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Welcome Speech</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Workshop</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>Workshop</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>Workshop</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>Briefing for Saturday
 (Room zzz)</t>
         </is>
       </c>
+      <c r="G3" s="1" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>10:15</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="3" t="inlineStr">
         <is>
           <t>Check in Maritime Museum
 Briefing for Saturday Concert 
@@ -527,154 +547,206 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>10:30</t>
         </is>
       </c>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="n"/>
+      <c r="E5" s="1" t="n"/>
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>10:45</t>
         </is>
       </c>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="n"/>
+      <c r="E6" s="1" t="n"/>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>Private Lesson with Ivy CHUANG 
 (Room Ivy)</t>
         </is>
       </c>
-      <c r="E7" s="2" t="inlineStr">
+      <c r="E7" s="3" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="F7" s="2" t="inlineStr">
+      <c r="F7" s="3" t="inlineStr">
         <is>
           <t>Flute MasterClass
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="G7" s="2" t="inlineStr">
+      <c r="G7" s="3" t="inlineStr">
         <is>
           <t>Rehearsal for Students and Friends Concert</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>11:15</t>
         </is>
       </c>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="n"/>
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" s="1" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>11:30</t>
         </is>
       </c>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>11:45</t>
         </is>
       </c>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
+      <c r="E10" s="1" t="n"/>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>12:00</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr">
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>Private Lesson with Ivy CHUANG 
 (Room Ivy)</t>
         </is>
       </c>
-      <c r="D11" s="2" t="inlineStr">
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>Rehearsal with pianist
 (Room Shelley)</t>
         </is>
       </c>
+      <c r="E11" s="1" t="n"/>
+      <c r="F11" s="1" t="n"/>
+      <c r="G11" s="1" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>12:15</t>
         </is>
       </c>
+      <c r="B12" s="1" t="n"/>
+      <c r="C12" s="1" t="n"/>
+      <c r="D12" s="1" t="n"/>
+      <c r="E12" s="1" t="n"/>
+      <c r="F12" s="1" t="n"/>
+      <c r="G12" s="1" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>12:30</t>
         </is>
       </c>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="n"/>
+      <c r="D13" s="1" t="n"/>
+      <c r="E13" s="1" t="n"/>
+      <c r="F13" s="1" t="n"/>
+      <c r="G13" s="1" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
         <is>
           <t>12:45</t>
         </is>
       </c>
+      <c r="B14" s="1" t="n"/>
+      <c r="C14" s="1" t="n"/>
+      <c r="D14" s="1" t="n"/>
+      <c r="E14" s="1" t="n"/>
+      <c r="F14" s="1" t="n"/>
+      <c r="G14" s="1" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="B15" s="2" t="inlineStr">
+      <c r="B15" s="3" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="C15" s="2" t="inlineStr">
+      <c r="C15" s="3" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr">
+      <c r="D15" s="3" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="E15" s="2" t="inlineStr">
+      <c r="E15" s="3" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="F15" s="2" t="inlineStr">
+      <c r="F15" s="3" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="G15" s="2" t="inlineStr">
+      <c r="G15" s="3" t="inlineStr">
         <is>
           <t>Lunch
 Dress Up, Warm Up</t>
@@ -682,152 +754,205 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>13:15</t>
         </is>
       </c>
+      <c r="B16" s="1" t="n"/>
+      <c r="C16" s="1" t="n"/>
+      <c r="D16" s="1" t="n"/>
+      <c r="E16" s="1" t="n"/>
+      <c r="F16" s="1" t="n"/>
+      <c r="G16" s="1" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="1" t="inlineStr">
         <is>
           <t>13:30</t>
         </is>
       </c>
+      <c r="B17" s="1" t="n"/>
+      <c r="C17" s="1" t="n"/>
+      <c r="D17" s="1" t="n"/>
+      <c r="E17" s="1" t="n"/>
+      <c r="F17" s="1" t="n"/>
+      <c r="G17" s="1" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="inlineStr">
         <is>
           <t>13:45</t>
         </is>
       </c>
+      <c r="B18" s="1" t="n"/>
+      <c r="C18" s="1" t="n"/>
+      <c r="D18" s="1" t="n"/>
+      <c r="E18" s="1" t="n"/>
+      <c r="F18" s="1" t="n"/>
+      <c r="G18" s="1" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="inlineStr">
         <is>
           <t>14:00</t>
         </is>
       </c>
-      <c r="B19" s="2" t="inlineStr">
+      <c r="B19" s="3" t="inlineStr">
         <is>
           <t>Private Lesson with Stephane RETY 
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="C19" s="2" t="inlineStr">
+      <c r="C19" s="3" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="D19" s="2" t="inlineStr">
+      <c r="D19" s="3" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="E19" s="2" t="inlineStr">
+      <c r="E19" s="3" t="inlineStr">
         <is>
           <t>Private Lesson with Stephane &amp; pianist 
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="F19" s="2" t="inlineStr">
+      <c r="F19" s="3" t="inlineStr">
         <is>
           <t>Flute MasterClass
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="G19" s="3" t="inlineStr">
+      <c r="G19" s="4" t="inlineStr">
         <is>
           <t>Concert call time</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="1" t="inlineStr">
         <is>
           <t>14:15</t>
         </is>
       </c>
-      <c r="G20" s="2" t="inlineStr">
+      <c r="B20" s="1" t="n"/>
+      <c r="C20" s="1" t="n"/>
+      <c r="D20" s="1" t="n"/>
+      <c r="E20" s="1" t="n"/>
+      <c r="F20" s="1" t="n"/>
+      <c r="G20" s="3" t="inlineStr">
         <is>
           <t>Lina Summer Camp of Music Students &amp; Friends Concert</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="1" t="inlineStr">
         <is>
           <t>14:30</t>
         </is>
       </c>
+      <c r="B21" s="1" t="n"/>
+      <c r="C21" s="1" t="n"/>
+      <c r="D21" s="1" t="n"/>
+      <c r="E21" s="1" t="n"/>
+      <c r="F21" s="1" t="n"/>
+      <c r="G21" s="1" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="1" t="inlineStr">
         <is>
           <t>14:45</t>
         </is>
       </c>
+      <c r="B22" s="1" t="n"/>
+      <c r="C22" s="1" t="n"/>
+      <c r="D22" s="1" t="n"/>
+      <c r="E22" s="1" t="n"/>
+      <c r="F22" s="1" t="n"/>
+      <c r="G22" s="1" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="1" t="inlineStr">
         <is>
           <t>15:00</t>
         </is>
       </c>
-      <c r="B23" s="2" t="inlineStr">
+      <c r="B23" s="3" t="inlineStr">
         <is>
           <t>Acting Class 
 (Room Acting)</t>
         </is>
       </c>
-      <c r="C23" s="2" t="inlineStr">
+      <c r="C23" s="3" t="inlineStr">
         <is>
           <t>Acting Class 
 (Room Acting)</t>
         </is>
       </c>
-      <c r="D23" s="2" t="inlineStr">
+      <c r="D23" s="3" t="inlineStr">
         <is>
           <t>Acting Class 
 (Room Acting)</t>
         </is>
       </c>
-      <c r="E23" s="2" t="inlineStr">
+      <c r="E23" s="3" t="inlineStr">
         <is>
           <t>Acting Class 
 (Room Acting)</t>
         </is>
       </c>
-      <c r="F23" s="2" t="inlineStr">
+      <c r="F23" s="3" t="inlineStr">
         <is>
           <t>Group Activity 
 (Room Group Activity)</t>
         </is>
       </c>
+      <c r="G23" s="1" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="1" t="inlineStr">
         <is>
           <t>15:15</t>
         </is>
       </c>
+      <c r="B24" s="1" t="n"/>
+      <c r="C24" s="1" t="n"/>
+      <c r="D24" s="1" t="n"/>
+      <c r="E24" s="1" t="n"/>
+      <c r="F24" s="1" t="n"/>
+      <c r="G24" s="1" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="1" t="inlineStr">
         <is>
           <t>15:30</t>
         </is>
       </c>
+      <c r="B25" s="1" t="n"/>
+      <c r="C25" s="1" t="n"/>
+      <c r="D25" s="1" t="n"/>
+      <c r="E25" s="1" t="n"/>
+      <c r="F25" s="1" t="n"/>
+      <c r="G25" s="1" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="1" t="inlineStr">
         <is>
           <t>15:45</t>
         </is>
       </c>
-      <c r="G26" s="2" t="inlineStr">
+      <c r="B26" s="1" t="n"/>
+      <c r="C26" s="1" t="n"/>
+      <c r="D26" s="1" t="n"/>
+      <c r="E26" s="1" t="n"/>
+      <c r="F26" s="1" t="n"/>
+      <c r="G26" s="3" t="inlineStr">
         <is>
           <t>After concert refreshment 
 (Maritime Museum)</t>
@@ -835,62 +960,81 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="1" t="inlineStr">
         <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="B27" s="2" t="inlineStr">
+      <c r="B27" s="3" t="inlineStr">
         <is>
           <t>Ensemble 
 (Room Tomasz)</t>
         </is>
       </c>
-      <c r="C27" s="2" t="inlineStr">
+      <c r="C27" s="3" t="inlineStr">
         <is>
           <t>Ensemble 
 (Room Tomasz)</t>
         </is>
       </c>
-      <c r="D27" s="2" t="inlineStr">
+      <c r="D27" s="3" t="inlineStr">
         <is>
           <t>Ensemble 
 (Room Tomasz)</t>
         </is>
       </c>
-      <c r="E27" s="2" t="inlineStr">
+      <c r="E27" s="3" t="inlineStr">
         <is>
           <t>Ensemble 
 (Room Tomasz)</t>
         </is>
       </c>
-      <c r="F27" s="2" t="inlineStr">
+      <c r="F27" s="3" t="inlineStr">
         <is>
           <t>Ensemble 
 (Room Tomasz)</t>
         </is>
       </c>
+      <c r="G27" s="1" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="1" t="inlineStr">
         <is>
           <t>16:15</t>
         </is>
       </c>
+      <c r="B28" s="1" t="n"/>
+      <c r="C28" s="1" t="n"/>
+      <c r="D28" s="1" t="n"/>
+      <c r="E28" s="1" t="n"/>
+      <c r="F28" s="1" t="n"/>
+      <c r="G28" s="1" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="1" t="inlineStr">
         <is>
           <t>16:30</t>
         </is>
       </c>
+      <c r="B29" s="1" t="n"/>
+      <c r="C29" s="1" t="n"/>
+      <c r="D29" s="1" t="n"/>
+      <c r="E29" s="1" t="n"/>
+      <c r="F29" s="1" t="n"/>
+      <c r="G29" s="1" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="1" t="inlineStr">
         <is>
           <t>16:45</t>
         </is>
       </c>
+      <c r="B30" s="1" t="n"/>
+      <c r="C30" s="1" t="n"/>
+      <c r="D30" s="1" t="n"/>
+      <c r="E30" s="1" t="n"/>
+      <c r="F30" s="1" t="n"/>
+      <c r="G30" s="1" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="37">

</xml_diff>

<commit_message>
Update date formatting in timetable generation to use full month names. Adjusted header text in both teacher and student timetable generation scripts for consistency.
</commit_message>
<xml_diff>
--- a/student_timetables/Cybi CHENG_timetable.xlsx
+++ b/student_timetables/Cybi CHENG_timetable.xlsx
@@ -451,32 +451,32 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>14 Jul (Monday)</t>
+          <t>14 July (Monday)</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>15 Jul (Tuesday)</t>
+          <t>15 July (Tuesday)</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>16 Jul (Wednesday)</t>
+          <t>16 July (Wednesday)</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>17 Jul (Thursday)</t>
+          <t>17 July (Thursday)</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>18 Jul (Friday)</t>
+          <t>18 July (Friday)</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>19 Jul (Saturday)</t>
+          <t>19 July (Saturday)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor timetable generation to apply consistent cell alignment and borders for improved visual presentation. Update alignment settings for both teacher and student timetables to center text and enable text wrapping.
</commit_message>
<xml_diff>
--- a/student_timetables/Cybi CHENG_timetable.xlsx
+++ b/student_timetables/Cybi CHENG_timetable.xlsx
@@ -55,15 +55,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,27 +497,27 @@
           <t>10:00</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>Welcome</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>Workshop</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D3" s="1" t="inlineStr">
         <is>
           <t>Workshop</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="E3" s="1" t="inlineStr">
         <is>
           <t>Workshop</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>Briefing for Saturday
 (Room zzz)</t>
@@ -538,7 +536,7 @@
       <c r="D4" s="1" t="n"/>
       <c r="E4" s="1" t="n"/>
       <c r="F4" s="1" t="n"/>
-      <c r="G4" s="3" t="inlineStr">
+      <c r="G4" s="1" t="inlineStr">
         <is>
           <t>Check in Maritime Museum
 Briefing for Saturday Concert 
@@ -578,37 +576,37 @@
           <t>11:00</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
+      <c r="D7" s="1" t="inlineStr">
         <is>
           <t>Private Lesson with Ivy CHUANG 
 (Room Ivy)</t>
         </is>
       </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E7" s="1" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="F7" s="1" t="inlineStr">
         <is>
           <t>Flute MasterClass
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="G7" s="3" t="inlineStr">
+      <c r="G7" s="1" t="inlineStr">
         <is>
           <t>Rehearsal for Students and Friends Concert</t>
         </is>
@@ -660,13 +658,13 @@
         </is>
       </c>
       <c r="B11" s="1" t="n"/>
-      <c r="C11" s="3" t="inlineStr">
+      <c r="C11" s="1" t="inlineStr">
         <is>
           <t>Private Lesson with Ivy CHUANG 
 (Room Ivy)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="D11" s="1" t="inlineStr">
         <is>
           <t>Rehearsal with pianist
 (Room Shelley)</t>
@@ -721,32 +719,32 @@
           <t>13:00</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr">
+      <c r="B15" s="1" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr">
+      <c r="C15" s="1" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="D15" s="3" t="inlineStr">
+      <c r="D15" s="1" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="E15" s="3" t="inlineStr">
+      <c r="E15" s="1" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="F15" s="3" t="inlineStr">
+      <c r="F15" s="1" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="G15" s="3" t="inlineStr">
+      <c r="G15" s="1" t="inlineStr">
         <is>
           <t>Lunch
 Dress Up, Warm Up</t>
@@ -798,41 +796,37 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B19" s="3" t="inlineStr">
+      <c r="B19" s="1" t="inlineStr">
         <is>
           <t>Private Lesson with Stephane RETY 
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="C19" s="3" t="inlineStr">
+      <c r="C19" s="1" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="D19" s="3" t="inlineStr">
+      <c r="D19" s="1" t="inlineStr">
         <is>
           <t>Practice 
 (Flute practice room)</t>
         </is>
       </c>
-      <c r="E19" s="3" t="inlineStr">
+      <c r="E19" s="1" t="inlineStr">
         <is>
           <t>Private Lesson with Stephane RETY &amp; pianist 
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="F19" s="3" t="inlineStr">
+      <c r="F19" s="1" t="inlineStr">
         <is>
           <t>Flute MasterClass
 (Room Stephane)</t>
         </is>
       </c>
-      <c r="G19" s="4" t="inlineStr">
-        <is>
-          <t>Concert call time</t>
-        </is>
-      </c>
+      <c r="G19" s="1" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -845,9 +839,9 @@
       <c r="D20" s="1" t="n"/>
       <c r="E20" s="1" t="n"/>
       <c r="F20" s="1" t="n"/>
-      <c r="G20" s="3" t="inlineStr">
-        <is>
-          <t>Lina Summer Camp of Music Students &amp; Friends Concert</t>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>Concert call time</t>
         </is>
       </c>
     </row>
@@ -862,7 +856,11 @@
       <c r="D21" s="1" t="n"/>
       <c r="E21" s="1" t="n"/>
       <c r="F21" s="1" t="n"/>
-      <c r="G21" s="1" t="n"/>
+      <c r="G21" s="1" t="inlineStr">
+        <is>
+          <t>Lina Summer Camp of Music Students &amp; Friends Concert</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -883,31 +881,31 @@
           <t>15:00</t>
         </is>
       </c>
-      <c r="B23" s="3" t="inlineStr">
+      <c r="B23" s="1" t="inlineStr">
         <is>
           <t>Acting Class 
 (Room Acting)</t>
         </is>
       </c>
-      <c r="C23" s="3" t="inlineStr">
+      <c r="C23" s="1" t="inlineStr">
         <is>
           <t>Acting Class 
 (Room Acting)</t>
         </is>
       </c>
-      <c r="D23" s="3" t="inlineStr">
+      <c r="D23" s="1" t="inlineStr">
         <is>
           <t>Acting Class 
 (Room Acting)</t>
         </is>
       </c>
-      <c r="E23" s="3" t="inlineStr">
+      <c r="E23" s="1" t="inlineStr">
         <is>
           <t>Acting Class 
 (Room Acting)</t>
         </is>
       </c>
-      <c r="F23" s="3" t="inlineStr">
+      <c r="F23" s="1" t="inlineStr">
         <is>
           <t>Group Activity 
 (Room Group Activity)</t>
@@ -952,50 +950,50 @@
       <c r="D26" s="1" t="n"/>
       <c r="E26" s="1" t="n"/>
       <c r="F26" s="1" t="n"/>
-      <c r="G26" s="3" t="inlineStr">
+      <c r="G26" s="1" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble 
+(Room Tomasz)</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble 
+(Room Tomasz)</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble 
+(Room Tomasz)</t>
+        </is>
+      </c>
+      <c r="E27" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble 
+(Room Tomasz)</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble 
+(Room Tomasz)</t>
+        </is>
+      </c>
+      <c r="G27" s="1" t="inlineStr">
         <is>
           <t>After concert refreshment 
 (Maritime Museum)</t>
         </is>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="B27" s="3" t="inlineStr">
-        <is>
-          <t>Ensemble 
-(Room Tomasz)</t>
-        </is>
-      </c>
-      <c r="C27" s="3" t="inlineStr">
-        <is>
-          <t>Ensemble 
-(Room Tomasz)</t>
-        </is>
-      </c>
-      <c r="D27" s="3" t="inlineStr">
-        <is>
-          <t>Ensemble 
-(Room Tomasz)</t>
-        </is>
-      </c>
-      <c r="E27" s="3" t="inlineStr">
-        <is>
-          <t>Ensemble 
-(Room Tomasz)</t>
-        </is>
-      </c>
-      <c r="F27" s="3" t="inlineStr">
-        <is>
-          <t>Ensemble 
-(Room Tomasz)</t>
-        </is>
-      </c>
-      <c r="G27" s="1" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -1040,6 +1038,7 @@
   <mergeCells count="37">
     <mergeCell ref="E7:E14"/>
     <mergeCell ref="E23:E26"/>
+    <mergeCell ref="G21:G26"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B14"/>
     <mergeCell ref="F15:F18"/>
@@ -1048,7 +1047,6 @@
     <mergeCell ref="D27:D30"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="G4:G6"/>
-    <mergeCell ref="G26:G28"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="F7:F14"/>
@@ -1056,7 +1054,6 @@
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="E15:E18"/>
     <mergeCell ref="B19:B22"/>
-    <mergeCell ref="G15:G18"/>
     <mergeCell ref="C27:C30"/>
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="E27:E30"/>
@@ -1069,12 +1066,13 @@
     <mergeCell ref="F27:F30"/>
     <mergeCell ref="C19:C22"/>
     <mergeCell ref="D23:D26"/>
-    <mergeCell ref="G20:G25"/>
+    <mergeCell ref="G27:G28"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="C15:C18"/>
     <mergeCell ref="D19:D22"/>
     <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G15:G19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove the generate_timetables.py script and outdated temporary files. Update student and teacher timetable files to reflect recent changes in timetable generation logic.
</commit_message>
<xml_diff>
--- a/student_timetables/Cybi CHENG_timetable.xlsx
+++ b/student_timetables/Cybi CHENG_timetable.xlsx
@@ -523,7 +523,13 @@
 (Room zzz)</t>
         </is>
       </c>
-      <c r="G3" s="1" t="n"/>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>Check in Maritime Museum
+Briefing for Saturday Concert
+Maritime Museum Tour</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -536,13 +542,7 @@
       <c r="D4" s="1" t="n"/>
       <c r="E4" s="1" t="n"/>
       <c r="F4" s="1" t="n"/>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>Check in Maritime Museum
-Briefing for Saturday Concert 
-Maritime Museum Tour</t>
-        </is>
-      </c>
+      <c r="G4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1019,7 +1019,7 @@
       <c r="D29" s="1" t="n"/>
       <c r="E29" s="1" t="n"/>
       <c r="F29" s="1" t="n"/>
-      <c r="G29" s="1" t="n"/>
+      <c r="G29" s="1" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -1035,7 +1035,7 @@
       <c r="G30" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="38">
     <mergeCell ref="E7:E14"/>
     <mergeCell ref="E23:E26"/>
     <mergeCell ref="G21:G26"/>
@@ -1046,10 +1046,10 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="D27:D30"/>
     <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G4:G6"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="F7:F14"/>
+    <mergeCell ref="G3:G6"/>
     <mergeCell ref="G7:G14"/>
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="E15:E18"/>
@@ -1057,6 +1057,7 @@
     <mergeCell ref="C27:C30"/>
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="E27:E30"/>
+    <mergeCell ref="G29:G30"/>
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="C11:C14"/>
     <mergeCell ref="B15:B18"/>

</xml_diff>